<commit_message>
Fixed R4R results / home load events
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-r4r.xlsx
+++ b/test-data/webanalytics-r4r.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CE3FA446-B499-46C2-8E21-BB6533E44282}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4CC65F2C-C7AA-4EEA-801B-3B8BAD7B5307}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Path</t>
   </si>
@@ -36,18 +36,6 @@
     <t>R4R Detail</t>
   </si>
   <si>
-    <t>/research/resources</t>
-  </si>
-  <si>
-    <t>R4R Home</t>
-  </si>
-  <si>
-    <t>/research/resources/search</t>
-  </si>
-  <si>
-    <t>R4R Results</t>
-  </si>
-  <si>
     <t>CustomText</t>
   </si>
   <si>
@@ -57,16 +45,10 @@
     <t>/research/resources/resource/2</t>
   </si>
   <si>
-    <t xml:space="preserve"> - National Cancer Institute</t>
-  </si>
-  <si>
     <t>: Next-Generation Clustered Heat Maps (NG-CHM) - National Cancer Institute</t>
   </si>
   <si>
     <t>: Enhancer Linking by Methylation/Expression Relationships (ELMER) - National Cancer Institute</t>
-  </si>
-  <si>
-    <t>: Search Results - National Cancer Institute</t>
   </si>
 </sst>
 </file>
@@ -434,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,51 +437,29 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Resource/Home page tests
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-r4r.xlsx
+++ b/test-data/webanalytics-r4r.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4CC65F2C-C7AA-4EEA-801B-3B8BAD7B5307}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3463E34F-A55F-4D65-8149-7F9070BFBFD7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="R4RPageLoad" sheetId="1" r:id="rId1"/>
+    <sheet name="R4RResourceLoad" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -45,10 +45,10 @@
     <t>/research/resources/resource/2</t>
   </si>
   <si>
-    <t>: Next-Generation Clustered Heat Maps (NG-CHM) - National Cancer Institute</t>
-  </si>
-  <si>
-    <t>: Enhancer Linking by Methylation/Expression Relationships (ELMER) - National Cancer Institute</t>
+    <t>Enhancer Linking by Methylation/Expression Relationships (ELMER) - National Cancer Institute</t>
+  </si>
+  <si>
+    <t>Next-Generation Clustered Heat Maps (NG-CHM) - National Cancer Institute</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored BeforeClass() for R4R wa pageloads
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-r4r.xlsx
+++ b/test-data/webanalytics-r4r.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3463E34F-A55F-4D65-8149-7F9070BFBFD7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{88EC9710-65BA-435D-B76F-FBD9B891CF18}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="R4RResourceLoad" sheetId="1" r:id="rId1"/>
+    <sheet name="R4RHomeLoad" sheetId="2" r:id="rId1"/>
+    <sheet name="R4RResultsLoad" sheetId="1" r:id="rId2"/>
+    <sheet name="R4RResourceLoad" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Path</t>
   </si>
@@ -49,6 +51,24 @@
   </si>
   <si>
     <t>Next-Generation Clustered Heat Maps (NG-CHM) - National Cancer Institute</t>
+  </si>
+  <si>
+    <t>/research/resources</t>
+  </si>
+  <si>
+    <t>R4R Home</t>
+  </si>
+  <si>
+    <t>/research/resources/search</t>
+  </si>
+  <si>
+    <t>R4R Results</t>
+  </si>
+  <si>
+    <t>/research/resources/resource/4</t>
+  </si>
+  <si>
+    <t>Driver-gene Inference by Genetical-Genomics and Information Theory (DIGGIT) - National Cancer Institute</t>
   </si>
 </sst>
 </file>
@@ -415,18 +435,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE37472-7E4E-485A-A848-E931A43AAC50}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="86.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538D913A-CBB4-4539-AF55-54A5D878FB3D}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="97.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -462,6 +554,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
OCEPROJECT-4912 - added load 'click' test for R4R results
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-r4r.xlsx
+++ b/test-data/webanalytics-r4r.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{88EC9710-65BA-435D-B76F-FBD9B891CF18}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F1003B1D-F47C-4E43-954C-DDDB052FC19C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="R4RHomeLoad" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Path</t>
   </si>
@@ -62,13 +62,61 @@
     <t>/research/resources/search</t>
   </si>
   <si>
-    <t>R4R Results</t>
-  </si>
-  <si>
     <t>/research/resources/resource/4</t>
   </si>
   <si>
     <t>Driver-gene Inference by Genetical-Genomics and Information Theory (DIGGIT) - National Cancer Institute</t>
+  </si>
+  <si>
+    <t>R4R Results (all)</t>
+  </si>
+  <si>
+    <t>R4R Results (tools)</t>
+  </si>
+  <si>
+    <t>R4R Results (areas)</t>
+  </si>
+  <si>
+    <t>R4R Results (filtered)</t>
+  </si>
+  <si>
+    <t>/research/resources/search?from=0&amp;toolTypes=analysis_tools</t>
+  </si>
+  <si>
+    <t>/research/resources/search?from=0&amp;researchAreas=cancer_omics</t>
+  </si>
+  <si>
+    <t>/research/resources/search?from=20&amp;toolSubtypes=modeling&amp;toolSubtypes=r_software&amp;toolTypes=analysis_tools</t>
+  </si>
+  <si>
+    <t>ActionStatus</t>
+  </si>
+  <si>
+    <t>Filters</t>
+  </si>
+  <si>
+    <t>r4r_results|view|none|ra=0;tt=0;rt=0;tst=0|1|</t>
+  </si>
+  <si>
+    <t>r4r_results|view|none|ra=0;tt=1;rt=0;tst=0|1|</t>
+  </si>
+  <si>
+    <t>r4r_results|view|none|ra=1;tt=0;rt=0;tst=0|1|</t>
+  </si>
+  <si>
+    <t>r4r_results|view|none|ra=0;tt=1;rt=0;tst=2|2|</t>
+  </si>
+  <si>
+    <t>modeling|r_software|analysis_tools</t>
+  </si>
+  <si>
+    <t>analysis_tools</t>
+  </si>
+  <si>
+    <t>cancer_omics</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -438,7 +486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE37472-7E4E-485A-A848-E931A43AAC50}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -472,32 +520,88 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="106.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -556,13 +660,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>